<commit_message>
Addition of findAgent, begining work on DTC inputs
</commit_message>
<xml_diff>
--- a/verification/kundurRamp/results/timings.xlsx
+++ b/verification/kundurRamp/results/timings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="14580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="14580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="gen trip 0" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1061,7 +1061,7 @@
   <dimension ref="B2:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>